<commit_message>
cleanups through 2008 and 2004 Refresh
</commit_message>
<xml_diff>
--- a/ope.ed.gov/2004/criminal-offenses-noncampus-virginia-colleges-and-universities-crime-2004.xlsx
+++ b/ope.ed.gov/2004/criminal-offenses-noncampus-virginia-colleges-and-universities-crime-2004.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet sheetId="1" name="Criminal_Offenses_Noncampus" state="visible" r:id="rId3"/>
+    <sheet sheetId="1" name="criminal-offenses-noncampus-vir" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,16 +13,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
-    <t>Criminal Offenses - Noncampus</t>
-  </si>
-  <si>
-    <t>Survey year</t>
-  </si>
-  <si>
-    <t>Unitid</t>
-  </si>
-  <si>
-    <t>Institution name</t>
+    <t>Survey Year</t>
+  </si>
+  <si>
+    <t>UnitID</t>
+  </si>
+  <si>
+    <t>Institution Name</t>
   </si>
   <si>
     <t>Campus ID</t>
@@ -34,28 +31,28 @@
     <t>Institution Size</t>
   </si>
   <si>
-    <t>Murder/Non-negligent manslaughter</t>
-  </si>
-  <si>
-    <t>Negligent manslaughter</t>
-  </si>
-  <si>
-    <t>Sex offenses - Forcible</t>
-  </si>
-  <si>
-    <t>Sex offenses - Non-forcible</t>
+    <t>Murder/Non-Negligent Manslaughter</t>
+  </si>
+  <si>
+    <t>Negligent Manslaughter</t>
+  </si>
+  <si>
+    <t>Sex Offenses - Forcible</t>
+  </si>
+  <si>
+    <t>Sex Offenses - Non-Forcible</t>
   </si>
   <si>
     <t>Robbery</t>
   </si>
   <si>
-    <t>Aggravated assault</t>
+    <t>Aggravated Assault</t>
   </si>
   <si>
     <t>Burglary</t>
   </si>
   <si>
-    <t>Motor vehicle theft</t>
+    <t>Motor Vehicle Theft</t>
   </si>
   <si>
     <t>Arson</t>
@@ -487,52 +484,94 @@
       <c t="s" s="1" r="A1">
         <v>0</v>
       </c>
+      <c t="s" s="1" r="B1">
+        <v>1</v>
+      </c>
+      <c t="s" s="1" r="C1">
+        <v>2</v>
+      </c>
+      <c t="s" s="1" r="D1">
+        <v>3</v>
+      </c>
+      <c t="s" s="1" r="E1">
+        <v>4</v>
+      </c>
+      <c t="s" s="1" r="F1">
+        <v>5</v>
+      </c>
+      <c t="s" s="1" r="G1">
+        <v>6</v>
+      </c>
+      <c t="s" s="1" r="H1">
+        <v>7</v>
+      </c>
+      <c t="s" s="1" r="I1">
+        <v>8</v>
+      </c>
+      <c t="s" s="1" r="J1">
+        <v>9</v>
+      </c>
+      <c t="s" s="1" r="K1">
+        <v>10</v>
+      </c>
+      <c t="s" s="1" r="L1">
+        <v>11</v>
+      </c>
+      <c t="s" s="1" r="M1">
+        <v>12</v>
+      </c>
+      <c t="s" s="1" r="N1">
+        <v>13</v>
+      </c>
+      <c t="s" s="1" r="O1">
+        <v>14</v>
+      </c>
     </row>
     <row r="2">
-      <c t="s" s="1" r="A2">
-        <v>1</v>
-      </c>
-      <c t="s" s="1" r="B2">
-        <v>2</v>
+      <c s="1" r="A2">
+        <v>2004.0</v>
+      </c>
+      <c s="1" r="B2">
+        <v>419022.0</v>
       </c>
       <c t="s" s="1" r="C2">
-        <v>3</v>
-      </c>
-      <c t="s" s="1" r="D2">
-        <v>4</v>
+        <v>15</v>
+      </c>
+      <c s="1" r="D2">
+        <v>1.0</v>
       </c>
       <c t="s" s="1" r="E2">
-        <v>5</v>
-      </c>
-      <c t="s" s="1" r="F2">
-        <v>6</v>
-      </c>
-      <c t="s" s="1" r="G2">
-        <v>7</v>
-      </c>
-      <c t="s" s="1" r="H2">
-        <v>8</v>
-      </c>
-      <c t="s" s="1" r="I2">
-        <v>9</v>
-      </c>
-      <c t="s" s="1" r="J2">
-        <v>10</v>
-      </c>
-      <c t="s" s="1" r="K2">
-        <v>11</v>
-      </c>
-      <c t="s" s="1" r="L2">
-        <v>12</v>
-      </c>
-      <c t="s" s="1" r="M2">
-        <v>13</v>
-      </c>
-      <c t="s" s="1" r="N2">
-        <v>14</v>
-      </c>
-      <c t="s" s="1" r="O2">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c s="1" r="F2">
+        <v>459.0</v>
+      </c>
+      <c s="1" r="G2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="H2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="I2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="J2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="K2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="L2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="M2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="N2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="O2">
+        <v>0.0</v>
       </c>
     </row>
     <row r="3">
@@ -543,13 +582,13 @@
         <v>419022.0</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c s="1" r="D3">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c t="s" s="1" r="E3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c s="1" r="F3">
         <v>459.0</v>
@@ -590,13 +629,13 @@
         <v>419022.0</v>
       </c>
       <c t="s" s="1" r="C4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c s="1" r="D4">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c t="s" s="1" r="E4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c s="1" r="F4">
         <v>459.0</v>
@@ -634,19 +673,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B5">
-        <v>419022.0</v>
+        <v>231420.0</v>
       </c>
       <c t="s" s="1" r="C5">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c s="1" r="D5">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c t="s" s="1" r="E5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c s="1" r="F5">
-        <v>459.0</v>
+        <v>2719.0</v>
       </c>
       <c s="1" r="G5">
         <v>0.0</v>
@@ -681,19 +720,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B6">
-        <v>231420.0</v>
+        <v>231536.0</v>
       </c>
       <c t="s" s="1" r="C6">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c s="1" r="D6">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c s="1" r="F6">
-        <v>2719.0</v>
+        <v>3942.0</v>
       </c>
       <c s="1" r="G6">
         <v>0.0</v>
@@ -728,19 +767,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B7">
-        <v>231536.0</v>
+        <v>231712.0</v>
       </c>
       <c t="s" s="1" r="C7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c s="1" r="D7">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c s="1" r="F7">
-        <v>3942.0</v>
+        <v>4681.0</v>
       </c>
       <c s="1" r="G7">
         <v>0.0</v>
@@ -775,19 +814,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B8">
-        <v>231712.0</v>
+        <v>231624.0</v>
       </c>
       <c t="s" s="1" r="C8">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c s="1" r="D8">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E8">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c s="1" r="F8">
-        <v>4681.0</v>
+        <v>7575.0</v>
       </c>
       <c s="1" r="G8">
         <v>0.0</v>
@@ -822,19 +861,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B9">
-        <v>231624.0</v>
+        <v>231882.0</v>
       </c>
       <c t="s" s="1" r="C9">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c s="1" r="D9">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E9">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c s="1" r="F9">
-        <v>7575.0</v>
+        <v>4060.0</v>
       </c>
       <c s="1" r="G9">
         <v>0.0</v>
@@ -869,19 +908,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B10">
-        <v>231882.0</v>
+        <v>232043.0</v>
       </c>
       <c t="s" s="1" r="C10">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c s="1" r="D10">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E10">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c s="1" r="F10">
-        <v>4060.0</v>
+        <v>1297.0</v>
       </c>
       <c s="1" r="G10">
         <v>0.0</v>
@@ -916,19 +955,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B11">
-        <v>232043.0</v>
+        <v>231970.0</v>
       </c>
       <c t="s" s="1" r="C11">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c s="1" r="D11">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E11">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c s="1" r="F11">
-        <v>1297.0</v>
+        <v>689.0</v>
       </c>
       <c s="1" r="G11">
         <v>0.0</v>
@@ -949,7 +988,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="M11">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="N11">
         <v>0.0</v>
@@ -963,19 +1002,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B12">
-        <v>231970.0</v>
+        <v>442806.0</v>
       </c>
       <c t="s" s="1" r="C12">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c s="1" r="D12">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E12">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c s="1" r="F12">
-        <v>689.0</v>
+        <v>306.0</v>
       </c>
       <c s="1" r="G12">
         <v>0.0</v>
@@ -996,7 +1035,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="M12">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="N12">
         <v>0.0</v>
@@ -1010,19 +1049,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B13">
-        <v>442806.0</v>
+        <v>232186.0</v>
       </c>
       <c t="s" s="1" r="C13">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c s="1" r="D13">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E13">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c s="1" r="F13">
-        <v>306.0</v>
+        <v>28874.0</v>
       </c>
       <c s="1" r="G13">
         <v>0.0</v>
@@ -1057,19 +1096,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B14">
-        <v>232186.0</v>
+        <v>232256.0</v>
       </c>
       <c t="s" s="1" r="C14">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c s="1" r="D14">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E14">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c s="1" r="F14">
-        <v>28874.0</v>
+        <v>1082.0</v>
       </c>
       <c s="1" r="G14">
         <v>0.0</v>
@@ -1104,19 +1143,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B15">
-        <v>232256.0</v>
+        <v>232265.0</v>
       </c>
       <c t="s" s="1" r="C15">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c s="1" r="D15">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E15">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c s="1" r="F15">
-        <v>1082.0</v>
+        <v>6154.0</v>
       </c>
       <c s="1" r="G15">
         <v>0.0</v>
@@ -1154,13 +1193,13 @@
         <v>232265.0</v>
       </c>
       <c t="s" s="1" r="C16">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c s="1" r="D16">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c t="s" s="1" r="E16">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c s="1" r="F16">
         <v>6154.0</v>
@@ -1201,13 +1240,13 @@
         <v>232265.0</v>
       </c>
       <c t="s" s="1" r="C17">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c s="1" r="D17">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c t="s" s="1" r="E17">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c s="1" r="F17">
         <v>6154.0</v>
@@ -1245,19 +1284,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B18">
-        <v>232265.0</v>
+        <v>232423.0</v>
       </c>
       <c t="s" s="1" r="C18">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c s="1" r="D18">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c t="s" s="1" r="E18">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c s="1" r="F18">
-        <v>6154.0</v>
+        <v>16108.0</v>
       </c>
       <c s="1" r="G18">
         <v>0.0</v>
@@ -1266,7 +1305,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I18">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c s="1" r="J18">
         <v>0.0</v>
@@ -1295,13 +1334,13 @@
         <v>232423.0</v>
       </c>
       <c t="s" s="1" r="C19">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c s="1" r="D19">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c t="s" s="1" r="E19">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c s="1" r="F19">
         <v>16108.0</v>
@@ -1313,7 +1352,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I19">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="J19">
         <v>0.0</v>
@@ -1339,19 +1378,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B20">
-        <v>232423.0</v>
+        <v>231837.0</v>
       </c>
       <c t="s" s="1" r="C20">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c s="1" r="D20">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c t="s" s="1" r="E20">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c s="1" r="F20">
-        <v>16108.0</v>
+        <v>744.0</v>
       </c>
       <c s="1" r="G20">
         <v>0.0</v>
@@ -1389,13 +1428,13 @@
         <v>231837.0</v>
       </c>
       <c t="s" s="1" r="C21">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c s="1" r="D21">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c t="s" s="1" r="E21">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c s="1" r="F21">
         <v>744.0</v>
@@ -1433,19 +1472,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B22">
-        <v>231837.0</v>
+        <v>232566.0</v>
       </c>
       <c t="s" s="1" r="C22">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c s="1" r="D22">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c t="s" s="1" r="E22">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c s="1" r="F22">
-        <v>744.0</v>
+        <v>4289.0</v>
       </c>
       <c s="1" r="G22">
         <v>0.0</v>
@@ -1480,19 +1519,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B23">
-        <v>232566.0</v>
+        <v>232575.0</v>
       </c>
       <c t="s" s="1" r="C23">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c s="1" r="D23">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E23">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c s="1" r="F23">
-        <v>4289.0</v>
+        <v>5416.0</v>
       </c>
       <c s="1" r="G23">
         <v>0.0</v>
@@ -1527,19 +1566,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B24">
-        <v>232575.0</v>
+        <v>232609.0</v>
       </c>
       <c t="s" s="1" r="C24">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c s="1" r="D24">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E24">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c s="1" r="F24">
-        <v>5416.0</v>
+        <v>2248.0</v>
       </c>
       <c s="1" r="G24">
         <v>0.0</v>
@@ -1574,19 +1613,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B25">
-        <v>232609.0</v>
+        <v>232788.0</v>
       </c>
       <c t="s" s="1" r="C25">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c s="1" r="D25">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E25">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c s="1" r="F25">
-        <v>2248.0</v>
+        <v>2906.0</v>
       </c>
       <c s="1" r="G25">
         <v>0.0</v>
@@ -1621,19 +1660,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B26">
-        <v>232788.0</v>
+        <v>232867.0</v>
       </c>
       <c t="s" s="1" r="C26">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c s="1" r="D26">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E26">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c s="1" r="F26">
-        <v>2906.0</v>
+        <v>4103.0</v>
       </c>
       <c s="1" r="G26">
         <v>0.0</v>
@@ -1668,19 +1707,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B27">
-        <v>232867.0</v>
+        <v>433299.0</v>
       </c>
       <c t="s" s="1" r="C27">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c s="1" r="D27">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E27">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c s="1" r="F27">
-        <v>4103.0</v>
+        <v>58.0</v>
       </c>
       <c s="1" r="G27">
         <v>0.0</v>
@@ -1715,19 +1754,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B28">
-        <v>433299.0</v>
+        <v>233417.0</v>
       </c>
       <c t="s" s="1" r="C28">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c s="1" r="D28">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E28">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c s="1" r="F28">
-        <v>58.0</v>
+        <v>56.0</v>
       </c>
       <c s="1" r="G28">
         <v>0.0</v>
@@ -1762,19 +1801,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B29">
-        <v>233417.0</v>
+        <v>232937.0</v>
       </c>
       <c t="s" s="1" r="C29">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c s="1" r="D29">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E29">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c s="1" r="F29">
-        <v>56.0</v>
+        <v>6165.0</v>
       </c>
       <c s="1" r="G29">
         <v>0.0</v>
@@ -1789,16 +1828,16 @@
         <v>0.0</v>
       </c>
       <c s="1" r="K29">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c s="1" r="L29">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="M29">
         <v>0.0</v>
       </c>
       <c s="1" r="N29">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c s="1" r="O29">
         <v>0.0</v>
@@ -1809,19 +1848,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B30">
-        <v>232937.0</v>
+        <v>232946.0</v>
       </c>
       <c t="s" s="1" r="C30">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c s="1" r="D30">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E30">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c s="1" r="F30">
-        <v>6165.0</v>
+        <v>37392.0</v>
       </c>
       <c s="1" r="G30">
         <v>0.0</v>
@@ -1836,16 +1875,16 @@
         <v>0.0</v>
       </c>
       <c s="1" r="K30">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="L30">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="M30">
         <v>0.0</v>
       </c>
       <c s="1" r="N30">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="O30">
         <v>0.0</v>
@@ -1859,13 +1898,13 @@
         <v>232946.0</v>
       </c>
       <c t="s" s="1" r="C31">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c s="1" r="D31">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c t="s" s="1" r="E31">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c s="1" r="F31">
         <v>37392.0</v>
@@ -1886,7 +1925,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L31">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c s="1" r="M31">
         <v>0.0</v>
@@ -1906,13 +1945,13 @@
         <v>232946.0</v>
       </c>
       <c t="s" s="1" r="C32">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c s="1" r="D32">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c t="s" s="1" r="E32">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c s="1" r="F32">
         <v>37392.0</v>
@@ -1933,7 +1972,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L32">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="M32">
         <v>0.0</v>
@@ -1953,13 +1992,13 @@
         <v>232946.0</v>
       </c>
       <c t="s" s="1" r="C33">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c s="1" r="D33">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c t="s" s="1" r="E33">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c s="1" r="F33">
         <v>37392.0</v>
@@ -2000,13 +2039,13 @@
         <v>232946.0</v>
       </c>
       <c t="s" s="1" r="C34">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c s="1" r="D34">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c t="s" s="1" r="E34">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c s="1" r="F34">
         <v>37392.0</v>
@@ -2044,19 +2083,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B35">
-        <v>232946.0</v>
+        <v>232982.0</v>
       </c>
       <c t="s" s="1" r="C35">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c s="1" r="D35">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
       <c t="s" s="1" r="E35">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c s="1" r="F35">
-        <v>37392.0</v>
+        <v>20595.0</v>
       </c>
       <c s="1" r="G35">
         <v>0.0</v>
@@ -2077,7 +2116,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="M35">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="N35">
         <v>0.0</v>
@@ -2091,19 +2130,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B36">
-        <v>232982.0</v>
+        <v>233019.0</v>
       </c>
       <c t="s" s="1" r="C36">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c s="1" r="D36">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E36">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c s="1" r="F36">
-        <v>20595.0</v>
+        <v>3341.0</v>
       </c>
       <c s="1" r="G36">
         <v>0.0</v>
@@ -2124,7 +2163,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="M36">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="N36">
         <v>0.0</v>
@@ -2138,19 +2177,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B37">
-        <v>233019.0</v>
+        <v>233116.0</v>
       </c>
       <c t="s" s="1" r="C37">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c s="1" r="D37">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E37">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c s="1" r="F37">
-        <v>3341.0</v>
+        <v>4358.0</v>
       </c>
       <c s="1" r="G37">
         <v>0.0</v>
@@ -2185,19 +2224,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B38">
-        <v>233116.0</v>
+        <v>233277.0</v>
       </c>
       <c t="s" s="1" r="C38">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c s="1" r="D38">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E38">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c s="1" r="F38">
-        <v>4358.0</v>
+        <v>9329.0</v>
       </c>
       <c s="1" r="G38">
         <v>0.0</v>
@@ -2206,7 +2245,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I38">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="J38">
         <v>0.0</v>
@@ -2232,19 +2271,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B39">
-        <v>233277.0</v>
+        <v>233301.0</v>
       </c>
       <c t="s" s="1" r="C39">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c s="1" r="D39">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E39">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c s="1" r="F39">
-        <v>9329.0</v>
+        <v>732.0</v>
       </c>
       <c s="1" r="G39">
         <v>0.0</v>
@@ -2253,7 +2292,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I39">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="J39">
         <v>0.0</v>
@@ -2279,19 +2318,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B40">
-        <v>233301.0</v>
+        <v>233408.0</v>
       </c>
       <c t="s" s="1" r="C40">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c s="1" r="D40">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E40">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c s="1" r="F40">
-        <v>732.0</v>
+        <v>155.0</v>
       </c>
       <c s="1" r="G40">
         <v>0.0</v>
@@ -2326,19 +2365,16 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B41">
-        <v>233408.0</v>
+        <v>435213.0</v>
       </c>
       <c t="s" s="1" r="C41">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c s="1" r="D41">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E41">
-        <v>93</v>
-      </c>
-      <c s="1" r="F41">
-        <v>155.0</v>
+        <v>94</v>
       </c>
       <c s="1" r="G41">
         <v>0.0</v>
@@ -2373,16 +2409,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B42">
-        <v>435213.0</v>
+        <v>233499.0</v>
       </c>
       <c t="s" s="1" r="C42">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c s="1" r="D42">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E42">
-        <v>95</v>
+        <v>96</v>
+      </c>
+      <c s="1" r="F42">
+        <v>627.0</v>
       </c>
       <c s="1" r="G42">
         <v>0.0</v>
@@ -2417,19 +2456,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B43">
-        <v>233499.0</v>
+        <v>233541.0</v>
       </c>
       <c t="s" s="1" r="C43">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c s="1" r="D43">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E43">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c s="1" r="F43">
-        <v>627.0</v>
+        <v>3000.0</v>
       </c>
       <c s="1" r="G43">
         <v>0.0</v>
@@ -2464,19 +2503,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B44">
-        <v>233541.0</v>
+        <v>233611.0</v>
       </c>
       <c t="s" s="1" r="C44">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c s="1" r="D44">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E44">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c s="1" r="F44">
-        <v>3000.0</v>
+        <v>581.0</v>
       </c>
       <c s="1" r="G44">
         <v>0.0</v>
@@ -2511,19 +2550,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B45">
-        <v>233611.0</v>
+        <v>233639.0</v>
       </c>
       <c t="s" s="1" r="C45">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c s="1" r="D45">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E45">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c s="1" r="F45">
-        <v>581.0</v>
+        <v>4686.0</v>
       </c>
       <c s="1" r="G45">
         <v>0.0</v>
@@ -2558,19 +2597,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B46">
-        <v>233639.0</v>
+        <v>440341.0</v>
       </c>
       <c t="s" s="1" r="C46">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c s="1" r="D46">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E46">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c s="1" r="F46">
-        <v>4686.0</v>
+        <v>958.0</v>
       </c>
       <c s="1" r="G46">
         <v>0.0</v>
@@ -2588,10 +2627,10 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L46">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="M46">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c s="1" r="N46">
         <v>0.0</v>
@@ -2605,19 +2644,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B47">
-        <v>440341.0</v>
+        <v>233897.0</v>
       </c>
       <c t="s" s="1" r="C47">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c s="1" r="D47">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E47">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c s="1" r="F47">
-        <v>958.0</v>
+        <v>1836.0</v>
       </c>
       <c s="1" r="G47">
         <v>0.0</v>
@@ -2635,10 +2674,10 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L47">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="M47">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="N47">
         <v>0.0</v>
@@ -2652,19 +2691,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B48">
-        <v>233897.0</v>
+        <v>233754.0</v>
       </c>
       <c t="s" s="1" r="C48">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c s="1" r="D48">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E48">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c s="1" r="F48">
-        <v>1836.0</v>
+        <v>8515.0</v>
       </c>
       <c s="1" r="G48">
         <v>0.0</v>
@@ -2699,19 +2738,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B49">
-        <v>233754.0</v>
+        <v>233772.0</v>
       </c>
       <c t="s" s="1" r="C49">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c s="1" r="D49">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c t="s" s="1" r="E49">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c s="1" r="F49">
-        <v>8515.0</v>
+        <v>22691.0</v>
       </c>
       <c s="1" r="G49">
         <v>0.0</v>
@@ -2732,7 +2771,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="M49">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="N49">
         <v>0.0</v>
@@ -2746,19 +2785,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B50">
-        <v>233772.0</v>
+        <v>232681.0</v>
       </c>
       <c t="s" s="1" r="C50">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c s="1" r="D50">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c t="s" s="1" r="E50">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c s="1" r="F50">
-        <v>22691.0</v>
+        <v>4729.0</v>
       </c>
       <c s="1" r="G50">
         <v>0.0</v>
@@ -2767,19 +2806,19 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I50">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="J50">
         <v>0.0</v>
       </c>
       <c s="1" r="K50">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="L50">
         <v>0.0</v>
       </c>
       <c s="1" r="M50">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="N50">
         <v>0.0</v>
@@ -2793,19 +2832,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B51">
-        <v>232681.0</v>
+        <v>233374.0</v>
       </c>
       <c t="s" s="1" r="C51">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c s="1" r="D51">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E51">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c s="1" r="F51">
-        <v>4729.0</v>
+        <v>4475.0</v>
       </c>
       <c s="1" r="G51">
         <v>0.0</v>
@@ -2814,13 +2853,13 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I51">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="J51">
         <v>0.0</v>
       </c>
       <c s="1" r="K51">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="L51">
         <v>0.0</v>
@@ -2840,19 +2879,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B52">
-        <v>233374.0</v>
+        <v>234076.0</v>
       </c>
       <c t="s" s="1" r="C52">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c s="1" r="D52">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E52">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c s="1" r="F52">
-        <v>4475.0</v>
+        <v>23341.0</v>
       </c>
       <c s="1" r="G52">
         <v>0.0</v>
@@ -2861,7 +2900,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I52">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c s="1" r="J52">
         <v>0.0</v>
@@ -2870,16 +2909,16 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L52">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c s="1" r="M52">
-        <v>0.0</v>
+        <v>16.0</v>
       </c>
       <c s="1" r="N52">
         <v>0.0</v>
       </c>
       <c s="1" r="O52">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="53">
@@ -2887,19 +2926,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B53">
-        <v>234076.0</v>
+        <v>234030.0</v>
       </c>
       <c t="s" s="1" r="C53">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c s="1" r="D53">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E53">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c s="1" r="F53">
-        <v>23341.0</v>
+        <v>28303.0</v>
       </c>
       <c s="1" r="G53">
         <v>0.0</v>
@@ -2908,7 +2947,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I53">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="J53">
         <v>0.0</v>
@@ -2917,16 +2956,16 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L53">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="M53">
-        <v>16.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="N53">
         <v>0.0</v>
       </c>
       <c s="1" r="O53">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="54">
@@ -2937,13 +2976,13 @@
         <v>234030.0</v>
       </c>
       <c t="s" s="1" r="C54">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c s="1" r="D54">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c t="s" s="1" r="E54">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c s="1" r="F54">
         <v>28303.0</v>
@@ -2981,19 +3020,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B55">
-        <v>234030.0</v>
+        <v>233912.0</v>
       </c>
       <c t="s" s="1" r="C55">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c s="1" r="D55">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c t="s" s="1" r="E55">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c s="1" r="F55">
-        <v>28303.0</v>
+        <v>1149.0</v>
       </c>
       <c s="1" r="G55">
         <v>0.0</v>
@@ -3028,19 +3067,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B56">
-        <v>233912.0</v>
+        <v>234085.0</v>
       </c>
       <c t="s" s="1" r="C56">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c s="1" r="D56">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E56">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c s="1" r="F56">
-        <v>1149.0</v>
+        <v>1362.0</v>
       </c>
       <c s="1" r="G56">
         <v>0.0</v>
@@ -3075,19 +3114,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B57">
-        <v>234085.0</v>
+        <v>233921.0</v>
       </c>
       <c t="s" s="1" r="C57">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c s="1" r="D57">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E57">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c s="1" r="F57">
-        <v>1362.0</v>
+        <v>27619.0</v>
       </c>
       <c s="1" r="G57">
         <v>0.0</v>
@@ -3108,10 +3147,10 @@
         <v>0.0</v>
       </c>
       <c s="1" r="M57">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c s="1" r="N57">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c s="1" r="O57">
         <v>0.0</v>
@@ -3122,19 +3161,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B58">
-        <v>233921.0</v>
+        <v>234155.0</v>
       </c>
       <c t="s" s="1" r="C58">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c s="1" r="D58">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E58">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c s="1" r="F58">
-        <v>27619.0</v>
+        <v>4859.0</v>
       </c>
       <c s="1" r="G58">
         <v>0.0</v>
@@ -3152,13 +3191,13 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L58">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c s="1" r="M58">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="N58">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="O58">
         <v>0.0</v>
@@ -3169,19 +3208,16 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B59">
-        <v>234155.0</v>
+        <v>234137.0</v>
       </c>
       <c t="s" s="1" r="C59">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c s="1" r="D59">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E59">
-        <v>129</v>
-      </c>
-      <c s="1" r="F59">
-        <v>4859.0</v>
+        <v>130</v>
       </c>
       <c s="1" r="G59">
         <v>0.0</v>
@@ -3199,7 +3235,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L59">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="M59">
         <v>0.0</v>
@@ -3216,16 +3252,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B60">
-        <v>234137.0</v>
+        <v>233949.0</v>
       </c>
       <c t="s" s="1" r="C60">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c s="1" r="D60">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E60">
-        <v>131</v>
+        <v>132</v>
+      </c>
+      <c s="1" r="F60">
+        <v>8361.0</v>
       </c>
       <c s="1" r="G60">
         <v>0.0</v>
@@ -3260,19 +3299,19 @@
         <v>2004.0</v>
       </c>
       <c s="1" r="B61">
-        <v>233949.0</v>
+        <v>234377.0</v>
       </c>
       <c t="s" s="1" r="C61">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c s="1" r="D61">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E61">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c s="1" r="F61">
-        <v>8361.0</v>
+        <v>2700.0</v>
       </c>
       <c s="1" r="G61">
         <v>0.0</v>
@@ -3299,53 +3338,6 @@
         <v>0.0</v>
       </c>
       <c s="1" r="O61">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="62">
-      <c s="1" r="A62">
-        <v>2004.0</v>
-      </c>
-      <c s="1" r="B62">
-        <v>234377.0</v>
-      </c>
-      <c t="s" s="1" r="C62">
-        <v>134</v>
-      </c>
-      <c s="1" r="D62">
-        <v>1.0</v>
-      </c>
-      <c t="s" s="1" r="E62">
-        <v>135</v>
-      </c>
-      <c s="1" r="F62">
-        <v>2700.0</v>
-      </c>
-      <c s="1" r="G62">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="H62">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="I62">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="J62">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="K62">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="L62">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="M62">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="N62">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="O62">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>